<commit_message>
Cleaning up project for 2024 GC data
</commit_message>
<xml_diff>
--- a/inputData/Copy of Exetainer Codes_02_27_2025.xlsx
+++ b/inputData/Copy of Exetainer Codes_02_27_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/beaulieu_jake_epa_gov/Documents/gitRepository/gas_lab/inputData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="117" documentId="13_ncr:1_{25711A3D-1CE6-4B1F-B61F-1929ABA5B0CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4A4B722-2619-4D14-AB44-3023E2FD2746}"/>
+  <xr:revisionPtr revIDLastSave="123" documentId="13_ncr:1_{25711A3D-1CE6-4B1F-B61F-1929ABA5B0CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C0A4F8E-4397-4CB6-B162-E7E969B3F40D}"/>
   <bookViews>
-    <workbookView xWindow="22944" yWindow="0" windowWidth="23232" windowHeight="18576" xr2:uid="{F0FE38C9-C1A4-44DF-9B0E-2691156D7FB2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="18696" xr2:uid="{F0FE38C9-C1A4-44DF-9B0E-2691156D7FB2}"/>
   </bookViews>
   <sheets>
     <sheet name="compare" sheetId="22" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2014" uniqueCount="673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2014" uniqueCount="674">
   <si>
     <t>F1</t>
   </si>
@@ -2037,9 +2037,6 @@
     <t>SG23.0816</t>
   </si>
   <si>
-    <t>not listed on gts</t>
-  </si>
-  <si>
     <t>PS240738</t>
   </si>
   <si>
@@ -2074,6 +2071,12 @@
   </si>
   <si>
     <t>PS24.1046</t>
+  </si>
+  <si>
+    <t>PS240557</t>
+  </si>
+  <si>
+    <t>PS240565</t>
   </si>
 </sst>
 </file>
@@ -2098,7 +2101,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2155,12 +2158,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2184,7 +2181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -2203,14 +2200,13 @@
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2545,8 +2541,8 @@
   <dimension ref="A1:I584"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A222" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E245" sqref="E245"/>
+      <pane ySplit="1" topLeftCell="A323" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C357" sqref="C357"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2574,718 +2570,718 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>570</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>666</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>666</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>570</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>667</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C3" s="13" t="s">
         <v>667</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
         <v>570</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B4" s="13" t="s">
+        <v>669</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>669</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>570</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>668</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C5" s="13" t="s">
         <v>668</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D5" s="17" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
-        <v>570</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>670</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>670</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
-        <v>570</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>669</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>669</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>570</v>
-      </c>
-    </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>578</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>579</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>580</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="20" t="s">
         <v>581</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="20" t="s">
         <v>582</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="20" t="s">
         <v>583</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="20" t="s">
         <v>584</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="20" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="20" t="s">
         <v>586</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="20" t="s">
         <v>587</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="20" t="s">
         <v>588</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="20" t="s">
         <v>589</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="20" t="s">
         <v>590</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="20" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="20" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="20" t="s">
         <v>593</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="20" t="s">
         <v>594</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="20" t="s">
         <v>595</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="20" t="s">
         <v>596</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="20" t="s">
         <v>597</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="20" t="s">
         <v>598</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="20" t="s">
         <v>599</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="20" t="s">
         <v>600</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="20" t="s">
         <v>601</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="20" t="s">
         <v>602</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="20" t="s">
         <v>603</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="20" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="20" t="s">
         <v>605</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="20" t="s">
         <v>606</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="20" t="s">
+      <c r="A35" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="20" t="s">
         <v>607</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="20" t="s">
         <v>608</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="20" t="s">
+      <c r="A37" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="20" t="s">
         <v>609</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="20" t="s">
+      <c r="A38" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="20" t="s">
         <v>610</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="20" t="s">
+      <c r="A39" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B39" s="21" t="s">
+      <c r="B39" s="20" t="s">
         <v>611</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="20" t="s">
+      <c r="A40" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B40" s="21" t="s">
+      <c r="B40" s="20" t="s">
         <v>612</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="20" t="s">
+      <c r="A41" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="20" t="s">
         <v>613</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="20" t="s">
+      <c r="A42" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="20" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="20" t="s">
+      <c r="A43" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B43" s="21" t="s">
+      <c r="B43" s="20" t="s">
         <v>615</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B44" s="21" t="s">
+      <c r="B44" s="20" t="s">
         <v>616</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="20" t="s">
+      <c r="A45" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B45" s="21" t="s">
+      <c r="B45" s="20" t="s">
         <v>617</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="20" t="s">
+      <c r="A46" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B46" s="21" t="s">
+      <c r="B46" s="20" t="s">
         <v>618</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="20" t="s">
+      <c r="A47" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B47" s="21" t="s">
+      <c r="B47" s="20" t="s">
         <v>619</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="20" t="s">
+      <c r="A48" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B48" s="21" t="s">
+      <c r="B48" s="20" t="s">
         <v>620</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="20" t="s">
+      <c r="A49" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B49" s="21" t="s">
+      <c r="B49" s="20" t="s">
         <v>621</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="20" t="s">
+      <c r="A50" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B50" s="21" t="s">
+      <c r="B50" s="20" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="20" t="s">
+      <c r="A51" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B51" s="21" t="s">
+      <c r="B51" s="20" t="s">
         <v>623</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="20" t="s">
+      <c r="A52" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B52" s="21" t="s">
+      <c r="B52" s="20" t="s">
         <v>624</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="20" t="s">
+      <c r="A53" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B53" s="21" t="s">
+      <c r="B53" s="20" t="s">
         <v>625</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="20" t="s">
+      <c r="A54" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B54" s="21" t="s">
+      <c r="B54" s="20" t="s">
         <v>626</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="20" t="s">
+      <c r="A55" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B55" s="21" t="s">
+      <c r="B55" s="20" t="s">
         <v>627</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B56" s="21" t="s">
+      <c r="B56" s="20" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="20" t="s">
+      <c r="A57" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B57" s="21" t="s">
+      <c r="B57" s="20" t="s">
         <v>629</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="20" t="s">
+      <c r="A58" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B58" s="21" t="s">
+      <c r="B58" s="20" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="20" t="s">
+      <c r="A59" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B59" s="21" t="s">
+      <c r="B59" s="20" t="s">
         <v>631</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="20" t="s">
+      <c r="A60" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B60" s="21" t="s">
+      <c r="B60" s="20" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="20" t="s">
+      <c r="A61" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B61" s="21" t="s">
+      <c r="B61" s="20" t="s">
         <v>633</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="20" t="s">
+      <c r="A62" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B62" s="21" t="s">
+      <c r="B62" s="20" t="s">
         <v>634</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="20" t="s">
+      <c r="A63" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B63" s="21" t="s">
+      <c r="B63" s="20" t="s">
         <v>635</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="20" t="s">
+      <c r="A64" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B64" s="21" t="s">
+      <c r="B64" s="20" t="s">
         <v>636</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="20" t="s">
+      <c r="A65" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B65" s="21" t="s">
+      <c r="B65" s="20" t="s">
         <v>637</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="20" t="s">
+      <c r="A66" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B66" s="21" t="s">
+      <c r="B66" s="20" t="s">
         <v>638</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="20" t="s">
+      <c r="A67" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B67" s="21" t="s">
+      <c r="B67" s="20" t="s">
         <v>639</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="20" t="s">
+      <c r="A68" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B68" s="21" t="s">
+      <c r="B68" s="20" t="s">
         <v>640</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="20" t="s">
+      <c r="A69" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B69" s="21" t="s">
+      <c r="B69" s="20" t="s">
         <v>641</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="20" t="s">
+      <c r="A70" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B70" s="21" t="s">
+      <c r="B70" s="20" t="s">
         <v>642</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="20" t="s">
+      <c r="A71" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B71" s="21" t="s">
+      <c r="B71" s="20" t="s">
         <v>643</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="20" t="s">
+      <c r="A72" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B72" s="21" t="s">
+      <c r="B72" s="20" t="s">
         <v>644</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="20" t="s">
+      <c r="A73" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B73" s="21" t="s">
+      <c r="B73" s="20" t="s">
         <v>645</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="20" t="s">
+      <c r="A74" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B74" s="21" t="s">
+      <c r="B74" s="20" t="s">
         <v>646</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="20" t="s">
+      <c r="A75" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B75" s="21" t="s">
+      <c r="B75" s="20" t="s">
         <v>647</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="20" t="s">
+      <c r="A76" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B76" s="21" t="s">
+      <c r="B76" s="20" t="s">
         <v>648</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="20" t="s">
+      <c r="A77" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B77" s="21" t="s">
+      <c r="B77" s="20" t="s">
         <v>649</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="20" t="s">
+      <c r="A78" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B78" s="21" t="s">
+      <c r="B78" s="20" t="s">
         <v>650</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="20" t="s">
+      <c r="A79" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B79" s="21" t="s">
+      <c r="B79" s="20" t="s">
         <v>651</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="20" t="s">
+      <c r="A80" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B80" s="21" t="s">
+      <c r="B80" s="20" t="s">
         <v>652</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="20" t="s">
+      <c r="A81" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B81" s="21" t="s">
+      <c r="B81" s="20" t="s">
         <v>653</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="20" t="s">
+      <c r="A82" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B82" s="21" t="s">
+      <c r="B82" s="20" t="s">
         <v>654</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="20" t="s">
+      <c r="A83" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B83" s="21" t="s">
+      <c r="B83" s="20" t="s">
         <v>655</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="20" t="s">
+      <c r="A84" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B84" s="21" t="s">
+      <c r="B84" s="20" t="s">
         <v>656</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="20" t="s">
+      <c r="A85" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B85" s="21" t="s">
+      <c r="B85" s="20" t="s">
         <v>657</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="20" t="s">
+      <c r="A86" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B86" s="21" t="s">
+      <c r="B86" s="20" t="s">
         <v>658</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="20" t="s">
+      <c r="A87" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="B87" s="22" t="s">
+      <c r="B87" s="21" t="s">
         <v>659</v>
       </c>
-      <c r="C87" s="15"/>
-      <c r="D87" s="18" t="s">
+      <c r="C87" s="14"/>
+      <c r="D87" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -3517,7 +3513,7 @@
       <c r="A116" s="12" t="s">
         <v>571</v>
       </c>
-      <c r="B116" s="19">
+      <c r="B116" s="18">
         <v>24.0029</v>
       </c>
       <c r="C116" t="s">
@@ -4509,13 +4505,13 @@
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A240" s="17" t="s">
+      <c r="A240" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B240" s="16">
+      <c r="B240" s="15">
         <v>24.032499999999999</v>
       </c>
-      <c r="C240" s="15" t="s">
+      <c r="C240" s="14" t="s">
         <v>476</v>
       </c>
     </row>
@@ -4526,7 +4522,7 @@
       <c r="B241" s="11">
         <v>24.032599999999999</v>
       </c>
-      <c r="C241" s="15" t="s">
+      <c r="C241" s="14" t="s">
         <v>486</v>
       </c>
     </row>
@@ -4537,7 +4533,7 @@
       <c r="B242" s="11">
         <v>24.032699999999998</v>
       </c>
-      <c r="C242" s="15" t="s">
+      <c r="C242" s="14" t="s">
         <v>487</v>
       </c>
     </row>
@@ -4548,7 +4544,7 @@
       <c r="B243" s="11">
         <v>24.032800000000002</v>
       </c>
-      <c r="C243" s="15" t="s">
+      <c r="C243" s="14" t="s">
         <v>488</v>
       </c>
     </row>
@@ -4559,7 +4555,7 @@
       <c r="B244" s="11">
         <v>24.032900000000001</v>
       </c>
-      <c r="C244" s="15" t="s">
+      <c r="C244" s="14" t="s">
         <v>485</v>
       </c>
     </row>
@@ -4570,29 +4566,29 @@
       <c r="B245" s="11">
         <v>24.033000000000001</v>
       </c>
-      <c r="C245" s="15" t="s">
+      <c r="C245" s="14" t="s">
         <v>479</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A246" s="17" t="s">
+      <c r="A246" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B246" s="16">
+      <c r="B246" s="15">
         <v>24.033100000000001</v>
       </c>
-      <c r="C246" s="15" t="s">
+      <c r="C246" s="14" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A247" s="17" t="s">
+      <c r="A247" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B247" s="16">
+      <c r="B247" s="15">
         <v>24.033200000000001</v>
       </c>
-      <c r="C247" s="15" t="s">
+      <c r="C247" s="14" t="s">
         <v>490</v>
       </c>
     </row>
@@ -4603,7 +4599,7 @@
       <c r="B248" s="11">
         <v>24.033300000000001</v>
       </c>
-      <c r="C248" s="15" t="s">
+      <c r="C248" s="14" t="s">
         <v>469</v>
       </c>
     </row>
@@ -4614,84 +4610,84 @@
       <c r="B249" s="11">
         <v>24.0334</v>
       </c>
-      <c r="C249" s="15" t="s">
+      <c r="C249" s="14" t="s">
         <v>470</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A250" s="17" t="s">
+      <c r="A250" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B250" s="16">
+      <c r="B250" s="15">
         <v>24.0335</v>
       </c>
-      <c r="C250" s="15" t="s">
+      <c r="C250" s="14" t="s">
         <v>474</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A251" s="17" t="s">
+      <c r="A251" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B251" s="16">
+      <c r="B251" s="15">
         <v>24.0336</v>
       </c>
-      <c r="C251" s="15" t="s">
+      <c r="C251" s="14" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A252" s="17" t="s">
+      <c r="A252" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B252" s="16">
+      <c r="B252" s="15">
         <v>24.0337</v>
       </c>
-      <c r="C252" s="15" t="s">
+      <c r="C252" s="14" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A253" s="17" t="s">
+      <c r="A253" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B253" s="16">
+      <c r="B253" s="15">
         <v>24.033799999999999</v>
       </c>
-      <c r="C253" s="15" t="s">
+      <c r="C253" s="14" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A254" s="17" t="s">
+      <c r="A254" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B254" s="16">
+      <c r="B254" s="15">
         <v>24.033899999999999</v>
       </c>
-      <c r="C254" s="15" t="s">
+      <c r="C254" s="14" t="s">
         <v>473</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A255" s="17" t="s">
+      <c r="A255" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B255" s="16">
+      <c r="B255" s="15">
         <v>24.033999999999999</v>
       </c>
-      <c r="C255" s="15" t="s">
+      <c r="C255" s="14" t="s">
         <v>482</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A256" s="17" t="s">
+      <c r="A256" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B256" s="16">
+      <c r="B256" s="15">
         <v>24.035299999999999</v>
       </c>
-      <c r="C256" s="15" t="s">
+      <c r="C256" s="14" t="s">
         <v>468</v>
       </c>
     </row>
@@ -5032,10 +5028,10 @@
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A299" s="17" t="s">
+      <c r="A299" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B299" s="16">
+      <c r="B299" s="15">
         <v>24.046900000000001</v>
       </c>
       <c r="C299" t="s">
@@ -5043,10 +5039,10 @@
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A300" s="17" t="s">
+      <c r="A300" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B300" s="16">
+      <c r="B300" s="15">
         <v>24.047000000000001</v>
       </c>
       <c r="C300" t="s">
@@ -5054,10 +5050,10 @@
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A301" s="17" t="s">
+      <c r="A301" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B301" s="16">
+      <c r="B301" s="15">
         <v>24.0471</v>
       </c>
       <c r="C301" t="s">
@@ -5065,10 +5061,10 @@
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A302" s="17" t="s">
+      <c r="A302" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B302" s="16">
+      <c r="B302" s="15">
         <v>24.0472</v>
       </c>
       <c r="C302" t="s">
@@ -5076,10 +5072,10 @@
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A303" s="17" t="s">
+      <c r="A303" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B303" s="16">
+      <c r="B303" s="15">
         <v>24.0473</v>
       </c>
       <c r="C303" t="s">
@@ -5087,10 +5083,10 @@
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A304" s="17" t="s">
+      <c r="A304" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B304" s="16">
+      <c r="B304" s="15">
         <v>24.0474</v>
       </c>
       <c r="C304" t="s">
@@ -5098,10 +5094,10 @@
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A305" s="17" t="s">
+      <c r="A305" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B305" s="16">
+      <c r="B305" s="15">
         <v>24.047499999999999</v>
       </c>
       <c r="C305" t="s">
@@ -5109,10 +5105,10 @@
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A306" s="17" t="s">
+      <c r="A306" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B306" s="16">
+      <c r="B306" s="15">
         <v>24.047599999999999</v>
       </c>
       <c r="C306" t="s">
@@ -5120,10 +5116,10 @@
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A307" s="17" t="s">
+      <c r="A307" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B307" s="16">
+      <c r="B307" s="15">
         <v>24.047699999999999</v>
       </c>
       <c r="C307" t="s">
@@ -5131,10 +5127,10 @@
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A308" s="17" t="s">
+      <c r="A308" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B308" s="16">
+      <c r="B308" s="15">
         <v>24.0505</v>
       </c>
       <c r="C308" t="s">
@@ -5142,10 +5138,10 @@
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A309" s="17" t="s">
+      <c r="A309" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B309" s="16">
+      <c r="B309" s="15">
         <v>24.050599999999999</v>
       </c>
       <c r="C309" t="s">
@@ -5153,10 +5149,10 @@
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A310" s="17" t="s">
+      <c r="A310" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B310" s="16">
+      <c r="B310" s="15">
         <v>24.050699999999999</v>
       </c>
       <c r="C310" t="s">
@@ -5164,10 +5160,10 @@
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A311" s="17" t="s">
+      <c r="A311" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B311" s="16">
+      <c r="B311" s="15">
         <v>24.050799999999999</v>
       </c>
       <c r="C311" t="s">
@@ -5175,10 +5171,10 @@
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A312" s="17" t="s">
+      <c r="A312" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B312" s="16">
+      <c r="B312" s="15">
         <v>24.050899999999999</v>
       </c>
       <c r="C312" t="s">
@@ -5186,10 +5182,10 @@
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A313" s="17" t="s">
+      <c r="A313" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B313" s="16">
+      <c r="B313" s="15">
         <v>24.050999999999998</v>
       </c>
       <c r="C313" t="s">
@@ -5197,10 +5193,10 @@
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A314" s="17" t="s">
+      <c r="A314" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B314" s="16">
+      <c r="B314" s="15">
         <v>24.051100000000002</v>
       </c>
       <c r="C314" t="s">
@@ -5208,10 +5204,10 @@
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A315" s="17" t="s">
+      <c r="A315" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B315" s="16">
+      <c r="B315" s="15">
         <v>24.051200000000001</v>
       </c>
       <c r="C315" t="s">
@@ -5219,10 +5215,10 @@
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A316" s="17" t="s">
+      <c r="A316" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B316" s="16">
+      <c r="B316" s="15">
         <v>24.051300000000001</v>
       </c>
       <c r="C316" t="s">
@@ -5230,10 +5226,10 @@
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A317" s="17" t="s">
+      <c r="A317" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B317" s="16">
+      <c r="B317" s="15">
         <v>24.051400000000001</v>
       </c>
       <c r="C317" t="s">
@@ -5241,10 +5237,10 @@
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A318" s="17" t="s">
+      <c r="A318" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B318" s="16">
+      <c r="B318" s="15">
         <v>24.051500000000001</v>
       </c>
       <c r="C318" t="s">
@@ -5252,10 +5248,10 @@
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A319" s="17" t="s">
+      <c r="A319" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B319" s="16">
+      <c r="B319" s="15">
         <v>24.051600000000001</v>
       </c>
       <c r="C319" t="s">
@@ -5263,10 +5259,10 @@
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A320" s="17" t="s">
+      <c r="A320" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B320" s="16">
+      <c r="B320" s="15">
         <v>24.052</v>
       </c>
       <c r="C320" t="s">
@@ -5274,10 +5270,10 @@
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A321" s="17" t="s">
+      <c r="A321" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B321" s="16">
+      <c r="B321" s="15">
         <v>24.052099999999999</v>
       </c>
       <c r="C321" t="s">
@@ -5285,10 +5281,10 @@
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A322" s="17" t="s">
+      <c r="A322" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B322" s="16">
+      <c r="B322" s="15">
         <v>24.052199999999999</v>
       </c>
       <c r="C322" t="s">
@@ -5296,10 +5292,10 @@
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A323" s="17" t="s">
+      <c r="A323" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B323" s="16">
+      <c r="B323" s="15">
         <v>24.052299999999999</v>
       </c>
       <c r="C323" t="s">
@@ -5307,10 +5303,10 @@
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A324" s="17" t="s">
+      <c r="A324" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B324" s="16">
+      <c r="B324" s="15">
         <v>24.052399999999999</v>
       </c>
       <c r="C324" t="s">
@@ -5318,10 +5314,10 @@
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A325" s="17" t="s">
+      <c r="A325" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B325" s="16">
+      <c r="B325" s="15">
         <v>24.052499999999998</v>
       </c>
       <c r="C325" t="s">
@@ -5329,10 +5325,10 @@
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A326" s="17" t="s">
+      <c r="A326" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B326" s="16">
+      <c r="B326" s="15">
         <v>24.052600000000002</v>
       </c>
       <c r="C326" t="s">
@@ -5340,10 +5336,10 @@
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A327" s="17" t="s">
+      <c r="A327" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B327" s="16">
+      <c r="B327" s="15">
         <v>24.052700000000002</v>
       </c>
       <c r="C327" t="s">
@@ -5351,10 +5347,10 @@
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A328" s="17" t="s">
+      <c r="A328" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B328" s="16">
+      <c r="B328" s="15">
         <v>24.052800000000001</v>
       </c>
       <c r="C328" t="s">
@@ -5362,10 +5358,10 @@
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A329" s="17" t="s">
+      <c r="A329" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B329" s="16">
+      <c r="B329" s="15">
         <v>24.052900000000001</v>
       </c>
       <c r="C329" t="s">
@@ -5373,10 +5369,10 @@
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A330" s="17" t="s">
+      <c r="A330" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B330" s="16">
+      <c r="B330" s="15">
         <v>24.053000000000001</v>
       </c>
       <c r="C330" t="s">
@@ -5384,10 +5380,10 @@
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A331" s="17" t="s">
+      <c r="A331" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B331" s="16">
+      <c r="B331" s="15">
         <v>24.053100000000001</v>
       </c>
       <c r="C331" t="s">
@@ -5395,10 +5391,10 @@
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A332" s="17" t="s">
+      <c r="A332" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B332" s="16">
+      <c r="B332" s="15">
         <v>24.0532</v>
       </c>
       <c r="C332" t="s">
@@ -5406,10 +5402,10 @@
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A333" s="17" t="s">
+      <c r="A333" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B333" s="16">
+      <c r="B333" s="15">
         <v>24.0533</v>
       </c>
       <c r="C333" t="s">
@@ -5417,10 +5413,10 @@
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A334" s="17" t="s">
+      <c r="A334" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B334" s="16">
+      <c r="B334" s="15">
         <v>24.0534</v>
       </c>
       <c r="C334" t="s">
@@ -5428,10 +5424,10 @@
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A335" s="17" t="s">
+      <c r="A335" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B335" s="16">
+      <c r="B335" s="15">
         <v>24.0535</v>
       </c>
       <c r="C335" t="s">
@@ -5439,10 +5435,10 @@
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A336" s="17" t="s">
+      <c r="A336" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B336" s="16">
+      <c r="B336" s="15">
         <v>24.053599999999999</v>
       </c>
       <c r="C336" t="s">
@@ -5450,10 +5446,10 @@
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A337" s="17" t="s">
+      <c r="A337" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B337" s="16">
+      <c r="B337" s="15">
         <v>24.053699999999999</v>
       </c>
       <c r="C337" t="s">
@@ -5461,10 +5457,10 @@
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A338" s="17" t="s">
+      <c r="A338" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B338" s="16">
+      <c r="B338" s="15">
         <v>24.053799999999999</v>
       </c>
       <c r="C338" t="s">
@@ -5472,10 +5468,10 @@
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A339" s="17" t="s">
+      <c r="A339" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B339" s="16">
+      <c r="B339" s="15">
         <v>24.053899999999999</v>
       </c>
       <c r="C339" t="s">
@@ -5483,10 +5479,10 @@
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A340" s="17" t="s">
+      <c r="A340" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B340" s="16">
+      <c r="B340" s="15">
         <v>24.053999999999998</v>
       </c>
       <c r="C340" t="s">
@@ -5494,10 +5490,10 @@
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A341" s="17" t="s">
+      <c r="A341" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B341" s="16">
+      <c r="B341" s="15">
         <v>24.054099999999998</v>
       </c>
       <c r="C341" t="s">
@@ -5505,10 +5501,10 @@
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A342" s="17" t="s">
+      <c r="A342" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B342" s="16">
+      <c r="B342" s="15">
         <v>24.054200000000002</v>
       </c>
       <c r="C342" t="s">
@@ -5516,10 +5512,10 @@
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A343" s="17" t="s">
+      <c r="A343" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B343" s="16">
+      <c r="B343" s="15">
         <v>24.054300000000001</v>
       </c>
       <c r="C343" t="s">
@@ -5527,10 +5523,10 @@
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A344" s="17" t="s">
+      <c r="A344" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B344" s="16">
+      <c r="B344" s="15">
         <v>24.054400000000001</v>
       </c>
       <c r="C344" t="s">
@@ -5538,10 +5534,10 @@
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A345" s="17" t="s">
+      <c r="A345" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B345" s="16">
+      <c r="B345" s="15">
         <v>24.054500000000001</v>
       </c>
       <c r="C345" t="s">
@@ -5549,10 +5545,10 @@
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A346" s="17" t="s">
+      <c r="A346" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B346" s="16">
+      <c r="B346" s="15">
         <v>24.054600000000001</v>
       </c>
       <c r="C346" t="s">
@@ -5560,10 +5556,10 @@
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A347" s="17" t="s">
+      <c r="A347" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B347" s="16">
+      <c r="B347" s="15">
         <v>24.0547</v>
       </c>
       <c r="C347" t="s">
@@ -5571,10 +5567,10 @@
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A348" s="17" t="s">
+      <c r="A348" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B348" s="16">
+      <c r="B348" s="15">
         <v>24.055399999999999</v>
       </c>
       <c r="C348" t="s">
@@ -5582,10 +5578,10 @@
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A349" s="17" t="s">
+      <c r="A349" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B349" s="16">
+      <c r="B349" s="15">
         <v>24.055499999999999</v>
       </c>
       <c r="C349" t="s">
@@ -5593,10 +5589,10 @@
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A350" s="17" t="s">
+      <c r="A350" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B350" s="16">
+      <c r="B350" s="15">
         <v>24.055599999999998</v>
       </c>
       <c r="C350" t="s">
@@ -5604,21 +5600,21 @@
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A351" s="17" t="s">
+      <c r="A351" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B351" s="16">
+      <c r="B351" s="15">
         <v>24.055700000000002</v>
       </c>
-      <c r="C351" s="14" t="s">
-        <v>660</v>
+      <c r="C351" t="s">
+        <v>672</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A352" s="17" t="s">
+      <c r="A352" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B352" s="16">
+      <c r="B352" s="15">
         <v>24.056100000000001</v>
       </c>
       <c r="C352" t="s">
@@ -5626,10 +5622,10 @@
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A353" s="17" t="s">
+      <c r="A353" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B353" s="16">
+      <c r="B353" s="15">
         <v>24.0562</v>
       </c>
       <c r="C353" t="s">
@@ -5637,10 +5633,10 @@
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A354" s="17" t="s">
+      <c r="A354" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B354" s="16">
+      <c r="B354" s="15">
         <v>24.0563</v>
       </c>
       <c r="C354" t="s">
@@ -5648,10 +5644,10 @@
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A355" s="17" t="s">
+      <c r="A355" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B355" s="16">
+      <c r="B355" s="15">
         <v>24.0564</v>
       </c>
       <c r="C355" t="s">
@@ -5659,21 +5655,21 @@
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A356" s="17" t="s">
+      <c r="A356" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B356" s="16">
+      <c r="B356" s="15">
         <v>24.0565</v>
       </c>
-      <c r="C356" s="14" t="s">
-        <v>660</v>
+      <c r="C356" t="s">
+        <v>673</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A357" s="17" t="s">
+      <c r="A357" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B357" s="16">
+      <c r="B357" s="15">
         <v>24.0566</v>
       </c>
       <c r="C357" t="s">
@@ -5681,10 +5677,10 @@
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A358" s="17" t="s">
+      <c r="A358" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B358" s="16">
+      <c r="B358" s="15">
         <v>24.056699999999999</v>
       </c>
       <c r="C358" t="s">
@@ -5692,10 +5688,10 @@
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A359" s="17" t="s">
+      <c r="A359" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B359" s="16">
+      <c r="B359" s="15">
         <v>24.056799999999999</v>
       </c>
       <c r="C359" t="s">
@@ -5703,10 +5699,10 @@
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A360" s="17" t="s">
+      <c r="A360" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B360" s="16">
+      <c r="B360" s="15">
         <v>24.056899999999999</v>
       </c>
       <c r="C360" t="s">
@@ -5714,10 +5710,10 @@
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A361" s="17" t="s">
+      <c r="A361" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B361" s="16">
+      <c r="B361" s="15">
         <v>24.056999999999999</v>
       </c>
       <c r="C361" t="s">
@@ -5725,10 +5721,10 @@
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A362" s="17" t="s">
+      <c r="A362" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B362" s="16">
+      <c r="B362" s="15">
         <v>24.057099999999998</v>
       </c>
       <c r="C362" t="s">
@@ -5736,10 +5732,10 @@
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A363" s="17" t="s">
+      <c r="A363" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B363" s="16">
+      <c r="B363" s="15">
         <v>24.057200000000002</v>
       </c>
       <c r="C363" t="s">
@@ -6062,8 +6058,8 @@
       <c r="B403" s="9">
         <v>24.073799999999999</v>
       </c>
-      <c r="C403" s="15" t="s">
-        <v>661</v>
+      <c r="C403" s="14" t="s">
+        <v>660</v>
       </c>
     </row>
     <row r="404" spans="2:3" x14ac:dyDescent="0.3">
@@ -6814,7 +6810,7 @@
       <c r="B490" s="9">
         <v>24.090900000000001</v>
       </c>
-      <c r="C490" s="15" t="s">
+      <c r="C490" s="14" t="s">
         <v>541</v>
       </c>
     </row>
@@ -6822,7 +6818,7 @@
       <c r="B491" s="9">
         <v>24.091000000000001</v>
       </c>
-      <c r="C491" s="15" t="s">
+      <c r="C491" s="14" t="s">
         <v>542</v>
       </c>
     </row>
@@ -6830,7 +6826,7 @@
       <c r="B492" s="9">
         <v>24.091100000000001</v>
       </c>
-      <c r="C492" s="15" t="s">
+      <c r="C492" s="14" t="s">
         <v>543</v>
       </c>
     </row>
@@ -6838,7 +6834,7 @@
       <c r="B493" s="9">
         <v>24.091200000000001</v>
       </c>
-      <c r="C493" s="15" t="s">
+      <c r="C493" s="14" t="s">
         <v>555</v>
       </c>
     </row>
@@ -6846,7 +6842,7 @@
       <c r="B494" s="9">
         <v>24.0913</v>
       </c>
-      <c r="C494" s="15" t="s">
+      <c r="C494" s="14" t="s">
         <v>554</v>
       </c>
     </row>
@@ -6854,7 +6850,7 @@
       <c r="B495" s="9">
         <v>24.0914</v>
       </c>
-      <c r="C495" s="15" t="s">
+      <c r="C495" s="14" t="s">
         <v>544</v>
       </c>
     </row>
@@ -6862,7 +6858,7 @@
       <c r="B496" s="9">
         <v>24.0915</v>
       </c>
-      <c r="C496" s="15" t="s">
+      <c r="C496" s="14" t="s">
         <v>545</v>
       </c>
     </row>
@@ -6870,16 +6866,16 @@
       <c r="B497" s="9">
         <v>24.0916</v>
       </c>
-      <c r="C497" s="15" t="s">
+      <c r="C497" s="14" t="s">
         <v>546</v>
       </c>
-      <c r="H497" s="15"/>
+      <c r="H497" s="14"/>
     </row>
     <row r="498" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B498" s="9">
         <v>24.091699999999999</v>
       </c>
-      <c r="C498" s="15" t="s">
+      <c r="C498" s="14" t="s">
         <v>556</v>
       </c>
     </row>
@@ -6887,7 +6883,7 @@
       <c r="B499" s="9">
         <v>24.091799999999999</v>
       </c>
-      <c r="C499" s="15" t="s">
+      <c r="C499" s="14" t="s">
         <v>557</v>
       </c>
     </row>
@@ -6895,7 +6891,7 @@
       <c r="B500" s="9">
         <v>24.091899999999999</v>
       </c>
-      <c r="C500" s="15" t="s">
+      <c r="C500" s="14" t="s">
         <v>553</v>
       </c>
     </row>
@@ -6903,7 +6899,7 @@
       <c r="B501" s="9">
         <v>24.091999999999999</v>
       </c>
-      <c r="C501" s="15" t="s">
+      <c r="C501" s="14" t="s">
         <v>552</v>
       </c>
     </row>
@@ -6911,7 +6907,7 @@
       <c r="B502" s="9">
         <v>24.092099999999999</v>
       </c>
-      <c r="C502" s="15" t="s">
+      <c r="C502" s="14" t="s">
         <v>550</v>
       </c>
     </row>
@@ -6919,7 +6915,7 @@
       <c r="B503" s="9">
         <v>24.092199999999998</v>
       </c>
-      <c r="C503" s="15" t="s">
+      <c r="C503" s="14" t="s">
         <v>551</v>
       </c>
     </row>
@@ -6928,14 +6924,14 @@
         <v>24.092300000000002</v>
       </c>
       <c r="C504" s="9" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="505" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B505" s="9">
         <v>24.092400000000001</v>
       </c>
-      <c r="C505" s="15" t="s">
+      <c r="C505" s="14" t="s">
         <v>558</v>
       </c>
     </row>
@@ -6943,7 +6939,7 @@
       <c r="B506" s="9">
         <v>24.092500000000001</v>
       </c>
-      <c r="C506" s="15" t="s">
+      <c r="C506" s="14" t="s">
         <v>559</v>
       </c>
     </row>
@@ -6951,7 +6947,7 @@
       <c r="B507" s="9">
         <v>24.092600000000001</v>
       </c>
-      <c r="C507" s="15" t="s">
+      <c r="C507" s="14" t="s">
         <v>547</v>
       </c>
     </row>
@@ -6959,7 +6955,7 @@
       <c r="B508" s="9">
         <v>24.092700000000001</v>
       </c>
-      <c r="C508" s="15" t="s">
+      <c r="C508" s="14" t="s">
         <v>548</v>
       </c>
     </row>
@@ -6967,10 +6963,10 @@
       <c r="B509" s="13">
         <v>24.1</v>
       </c>
-      <c r="C509" s="15" t="s">
-        <v>671</v>
-      </c>
-      <c r="D509" s="18" t="s">
+      <c r="C509" s="14" t="s">
+        <v>670</v>
+      </c>
+      <c r="D509" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -6978,10 +6974,10 @@
       <c r="B510" s="13">
         <v>24.1004</v>
       </c>
-      <c r="C510" s="15" t="s">
+      <c r="C510" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="D510" s="18" t="s">
+      <c r="D510" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -6989,10 +6985,10 @@
       <c r="B511" s="13">
         <v>24.1005</v>
       </c>
-      <c r="C511" s="15" t="s">
+      <c r="C511" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="D511" s="18" t="s">
+      <c r="D511" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7000,10 +6996,10 @@
       <c r="B512" s="13">
         <v>24.1006</v>
       </c>
-      <c r="C512" s="15" t="s">
+      <c r="C512" s="14" t="s">
         <v>478</v>
       </c>
-      <c r="D512" s="18" t="s">
+      <c r="D512" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7011,10 +7007,10 @@
       <c r="B513" s="13">
         <v>24.101199999999999</v>
       </c>
-      <c r="C513" s="15" t="s">
+      <c r="C513" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="D513" s="18" t="s">
+      <c r="D513" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7022,10 +7018,10 @@
       <c r="B514" s="13">
         <v>24.101400000000002</v>
       </c>
-      <c r="C514" s="15" t="s">
+      <c r="C514" s="14" t="s">
         <v>480</v>
       </c>
-      <c r="D514" s="18" t="s">
+      <c r="D514" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7033,10 +7029,10 @@
       <c r="B515" s="13">
         <v>24.101500000000001</v>
       </c>
-      <c r="C515" s="15" t="s">
+      <c r="C515" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="D515" s="18" t="s">
+      <c r="D515" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7044,10 +7040,10 @@
       <c r="B516" s="13">
         <v>24.101700000000001</v>
       </c>
-      <c r="C516" s="15" t="s">
+      <c r="C516" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="D516" s="18" t="s">
+      <c r="D516" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7055,10 +7051,10 @@
       <c r="B517" s="13">
         <v>24.101900000000001</v>
       </c>
-      <c r="C517" s="15" t="s">
+      <c r="C517" s="14" t="s">
         <v>266</v>
       </c>
-      <c r="D517" s="18" t="s">
+      <c r="D517" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7066,10 +7062,10 @@
       <c r="B518" s="13">
         <v>24.1021</v>
       </c>
-      <c r="C518" s="15" t="s">
+      <c r="C518" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="D518" s="18" t="s">
+      <c r="D518" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7077,10 +7073,10 @@
       <c r="B519" s="13">
         <v>24.1023</v>
       </c>
-      <c r="C519" s="15" t="s">
+      <c r="C519" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="D519" s="18" t="s">
+      <c r="D519" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7088,10 +7084,10 @@
       <c r="B520" s="13">
         <v>24.102399999999999</v>
       </c>
-      <c r="C520" s="15" t="s">
+      <c r="C520" s="14" t="s">
         <v>505</v>
       </c>
-      <c r="D520" s="18" t="s">
+      <c r="D520" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7099,10 +7095,10 @@
       <c r="B521" s="13">
         <v>24.102799999999998</v>
       </c>
-      <c r="C521" s="15" t="s">
+      <c r="C521" s="14" t="s">
         <v>372</v>
       </c>
-      <c r="D521" s="18" t="s">
+      <c r="D521" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7110,10 +7106,10 @@
       <c r="B522" s="13">
         <v>24.102900000000002</v>
       </c>
-      <c r="C522" s="15" t="s">
+      <c r="C522" s="14" t="s">
         <v>477</v>
       </c>
-      <c r="D522" s="18" t="s">
+      <c r="D522" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7124,7 +7120,7 @@
       <c r="C523" t="s">
         <v>234</v>
       </c>
-      <c r="D523" s="18" t="s">
+      <c r="D523" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7135,7 +7131,7 @@
       <c r="C524" t="s">
         <v>410</v>
       </c>
-      <c r="D524" s="18" t="s">
+      <c r="D524" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7146,7 +7142,7 @@
       <c r="C525" t="s">
         <v>265</v>
       </c>
-      <c r="D525" s="18" t="s">
+      <c r="D525" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7157,7 +7153,7 @@
       <c r="C526" t="s">
         <v>344</v>
       </c>
-      <c r="D526" s="18" t="s">
+      <c r="D526" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7168,7 +7164,7 @@
       <c r="C527" t="s">
         <v>363</v>
       </c>
-      <c r="D527" s="18" t="s">
+      <c r="D527" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7179,7 +7175,7 @@
       <c r="C528" t="s">
         <v>297</v>
       </c>
-      <c r="D528" s="18" t="s">
+      <c r="D528" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7190,21 +7186,21 @@
       <c r="C529" t="s">
         <v>190</v>
       </c>
-      <c r="D529" s="18" t="s">
+      <c r="D529" s="17" t="s">
         <v>570</v>
       </c>
     </row>
     <row r="530" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A530" s="20" t="s">
+      <c r="A530" s="19" t="s">
         <v>572</v>
       </c>
       <c r="B530" s="13" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C530" s="13" t="s">
-        <v>672</v>
-      </c>
-      <c r="D530" s="18" t="s">
+        <v>671</v>
+      </c>
+      <c r="D530" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7215,7 +7211,7 @@
       <c r="C531" t="s">
         <v>298</v>
       </c>
-      <c r="D531" s="18" t="s">
+      <c r="D531" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7226,7 +7222,7 @@
       <c r="C532" t="s">
         <v>210</v>
       </c>
-      <c r="D532" s="18" t="s">
+      <c r="D532" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7235,9 +7231,9 @@
         <v>24.105899999999998</v>
       </c>
       <c r="C533" t="s">
-        <v>663</v>
-      </c>
-      <c r="D533" s="18" t="s">
+        <v>662</v>
+      </c>
+      <c r="D533" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7248,7 +7244,7 @@
       <c r="C534" t="s">
         <v>131</v>
       </c>
-      <c r="D534" s="18" t="s">
+      <c r="D534" s="17" t="s">
         <v>570</v>
       </c>
       <c r="E534" t="s">
@@ -7262,7 +7258,7 @@
       <c r="C535" t="s">
         <v>35</v>
       </c>
-      <c r="D535" s="18" t="s">
+      <c r="D535" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7281,7 +7277,7 @@
       <c r="C537" t="s">
         <v>289</v>
       </c>
-      <c r="D537" s="18" t="s">
+      <c r="D537" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7292,7 +7288,7 @@
       <c r="C538" t="s">
         <v>263</v>
       </c>
-      <c r="D538" s="18" t="s">
+      <c r="D538" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7300,10 +7296,10 @@
       <c r="B539" s="13">
         <v>24.107500000000002</v>
       </c>
-      <c r="C539" s="15" t="s">
+      <c r="C539" s="14" t="s">
         <v>484</v>
       </c>
-      <c r="D539" s="18" t="s">
+      <c r="D539" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7314,7 +7310,7 @@
       <c r="C540" t="s">
         <v>573</v>
       </c>
-      <c r="D540" s="18" t="s">
+      <c r="D540" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7325,7 +7321,7 @@
       <c r="C541" t="s">
         <v>374</v>
       </c>
-      <c r="D541" s="18" t="s">
+      <c r="D541" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7336,7 +7332,7 @@
       <c r="C542" t="s">
         <v>144</v>
       </c>
-      <c r="D542" s="18" t="s">
+      <c r="D542" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7344,10 +7340,10 @@
       <c r="B543" s="13">
         <v>24.108000000000001</v>
       </c>
-      <c r="C543" s="15" t="s">
+      <c r="C543" s="14" t="s">
         <v>483</v>
       </c>
-      <c r="D543" s="18" t="s">
+      <c r="D543" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7358,7 +7354,7 @@
       <c r="C544" t="s">
         <v>132</v>
       </c>
-      <c r="D544" s="18" t="s">
+      <c r="D544" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7369,7 +7365,7 @@
       <c r="C545" t="s">
         <v>47</v>
       </c>
-      <c r="D545" s="18" t="s">
+      <c r="D545" s="17" t="s">
         <v>570</v>
       </c>
     </row>
@@ -7711,20 +7707,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -7827,7 +7823,7 @@
         <v>290</v>
       </c>
       <c r="F8" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="H8" t="s">
         <v>291</v>
@@ -7939,20 +7935,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -8249,20 +8245,20 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -8495,20 +8491,20 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -8736,20 +8732,20 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -8880,7 +8876,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -8983,26 +8979,26 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -9072,7 +9068,7 @@
         <v>423</v>
       </c>
       <c r="F5" t="s">
-        <v>116</v>
+        <v>672</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -9223,7 +9219,7 @@
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>415</v>
+        <v>673</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -9264,20 +9260,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -9596,20 +9592,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -9740,8 +9736,8 @@
       <c r="F9" t="s">
         <v>507</v>
       </c>
-      <c r="H9" s="15" t="s">
-        <v>671</v>
+      <c r="H9" s="14" t="s">
+        <v>670</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -9882,20 +9878,20 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -9954,7 +9950,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -10001,7 +9997,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -10026,7 +10022,7 @@
         <v>534</v>
       </c>
       <c r="H10" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -10126,20 +10122,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -10480,32 +10476,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="25" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="26" t="s">
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="R1" s="26"/>
+      <c r="R1" s="25"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -10831,20 +10827,20 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -11120,7 +11116,7 @@
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -11170,32 +11166,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="25" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="26" t="s">
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="R1" s="26"/>
+      <c r="R1" s="25"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -11555,32 +11551,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="25" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="26" t="s">
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="R1" s="26"/>
+      <c r="R1" s="25"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -11880,32 +11876,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="25" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="26" t="s">
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="R1" s="26"/>
+      <c r="R1" s="25"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -12115,32 +12111,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="25" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="26" t="s">
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="R1" s="26"/>
+      <c r="R1" s="25"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -12465,32 +12461,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="25" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="26" t="s">
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="R1" s="26"/>
+      <c r="R1" s="25"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -12778,32 +12774,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="25" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="26" t="s">
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="R1" s="26"/>
+      <c r="R1" s="25"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -13130,32 +13126,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="25" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="26" t="s">
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="R1" s="26"/>
+      <c r="R1" s="25"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -13444,6 +13440,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B32B05FB6ADEDD4FA21CF4AC8A21948D" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e697188abcb4d9c7a91b3e6db26b615e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="6a95d896-06a3-430a-9971-f8c7ad9f8a81" xmlns:ns6="69c4b106-11c4-44cf-8723-51008b5d0adb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9d0b3beaea61c81ce1dd18bb38314f1f" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -13894,7 +13895,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
@@ -13936,7 +13937,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -13945,12 +13946,15 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A991D51-407A-434F-845E-800E89EB4F21}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F17EF4C5-5033-4169-881B-588DA9EFC111}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13973,7 +13977,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87AFE480-2B2F-4C18-AC4B-3392EFE8E1E6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -13987,18 +13991,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E338E5E9-2850-47A6-9C67-2011EB9C67DD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A991D51-407A-434F-845E-800E89EB4F21}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>